<commit_message>
add location label cu in file location_PG
</commit_message>
<xml_diff>
--- a/_linhtinh/file_linhtinh/location_PG.xlsx
+++ b/_linhtinh/file_linhtinh/location_PG.xlsx
@@ -8,35 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\P&amp;G\my_project\_linhtinh\file_linhtinh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E78D21-2E7C-4C04-AD3F-EAE069D9EDD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E0CFA3-C9C7-41C5-9CFF-DF4E2188C71A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="3" xr2:uid="{4D41C987-C583-498E-A0D5-2638ABE40D36}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="27852" windowHeight="16416" activeTab="3" xr2:uid="{4D41C987-C583-498E-A0D5-2638ABE40D36}"/>
   </bookViews>
   <sheets>
     <sheet name="WH2" sheetId="1" r:id="rId1"/>
     <sheet name="WH3" sheetId="2" r:id="rId2"/>
     <sheet name="WH1" sheetId="3" r:id="rId3"/>
-    <sheet name="LABEL" sheetId="4" r:id="rId4"/>
-    <sheet name="CL3" sheetId="5" r:id="rId5"/>
-    <sheet name="CL1" sheetId="6" r:id="rId6"/>
-    <sheet name="CL2" sheetId="7" r:id="rId7"/>
-    <sheet name="PF5" sheetId="8" r:id="rId8"/>
-    <sheet name="PF4" sheetId="10" r:id="rId9"/>
-    <sheet name="PF3" sheetId="11" r:id="rId10"/>
-    <sheet name="PF2" sheetId="12" r:id="rId11"/>
-    <sheet name="PF1" sheetId="13" r:id="rId12"/>
+    <sheet name="LABEL_OLD" sheetId="14" r:id="rId4"/>
+    <sheet name="LABEL" sheetId="4" r:id="rId5"/>
+    <sheet name="CL3" sheetId="5" r:id="rId6"/>
+    <sheet name="CL1" sheetId="6" r:id="rId7"/>
+    <sheet name="CL2" sheetId="7" r:id="rId8"/>
+    <sheet name="PF5" sheetId="8" r:id="rId9"/>
+    <sheet name="PF4" sheetId="10" r:id="rId10"/>
+    <sheet name="PF3" sheetId="11" r:id="rId11"/>
+    <sheet name="PF2" sheetId="12" r:id="rId12"/>
+    <sheet name="PF1" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'CL1'!$A$1:$D$25</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'CL2'!$A$1:$D$63</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CL3'!$A$1:$D$44</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'PF1'!$A$1:$E$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'PF2'!$A$1:$E$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'PF3'!$A$1:$E$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'PF4'!$A$1:$E$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'PF5'!$A$1:$E$156</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'CL1'!$A$1:$D$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'CL2'!$A$1:$D$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'CL3'!$A$1:$D$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'PF1'!$A$1:$E$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'PF2'!$A$1:$E$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'PF3'!$A$1:$E$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'PF4'!$A$1:$E$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'PF5'!$A$1:$E$156</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,12 +45,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -307,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="599">
   <si>
     <t>STT</t>
   </si>
@@ -2095,6 +2091,15 @@
   </si>
   <si>
     <t>FZ112</t>
+  </si>
+  <si>
+    <t>LB1</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>LB2</t>
   </si>
 </sst>
 </file>
@@ -2989,6 +2994,674 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A7EB63-AF35-4A34-A800-1BC5F8A1BD55}">
+  <dimension ref="A1:J53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f t="shared" ref="A2:A33" si="0">ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>502</v>
+      </c>
+      <c r="E3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>503</v>
+      </c>
+      <c r="E4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>504</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>505</v>
+      </c>
+      <c r="E6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>506</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>508</v>
+      </c>
+      <c r="E9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>457</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>473</v>
+      </c>
+      <c r="E11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>489</v>
+      </c>
+      <c r="E12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>458</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>474</v>
+      </c>
+      <c r="E14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>490</v>
+      </c>
+      <c r="E15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>459</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>475</v>
+      </c>
+      <c r="E17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>491</v>
+      </c>
+      <c r="E18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>460</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>476</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>492</v>
+      </c>
+      <c r="E21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>461</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>477</v>
+      </c>
+      <c r="E23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>493</v>
+      </c>
+      <c r="E24">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>462</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>478</v>
+      </c>
+      <c r="E26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>494</v>
+      </c>
+      <c r="E27">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>463</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>479</v>
+      </c>
+      <c r="E29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>495</v>
+      </c>
+      <c r="E30">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>464</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>480</v>
+      </c>
+      <c r="E32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>496</v>
+      </c>
+      <c r="E33">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" ref="A34:A53" si="1">ROW()-1</f>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>465</v>
+      </c>
+      <c r="E34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>481</v>
+      </c>
+      <c r="E35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>466</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>482</v>
+      </c>
+      <c r="E37">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>467</v>
+      </c>
+      <c r="E38">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>483</v>
+      </c>
+      <c r="E39">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>468</v>
+      </c>
+      <c r="E40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>484</v>
+      </c>
+      <c r="E41">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>469</v>
+      </c>
+      <c r="E42">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>485</v>
+      </c>
+      <c r="E43">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>497</v>
+      </c>
+      <c r="E44">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>470</v>
+      </c>
+      <c r="E45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>486</v>
+      </c>
+      <c r="E46">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>498</v>
+      </c>
+      <c r="E47">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>471</v>
+      </c>
+      <c r="E48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>487</v>
+      </c>
+      <c r="E49">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>499</v>
+      </c>
+      <c r="E50">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>472</v>
+      </c>
+      <c r="E51">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>488</v>
+      </c>
+      <c r="E52">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>500</v>
+      </c>
+      <c r="E53">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E53" xr:uid="{35A7EB63-AF35-4A34-A800-1BC5F8A1BD55}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E53">
+      <sortCondition ref="B1:B53"/>
+    </sortState>
+  </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6042DF-4EBE-4EA9-8D04-2EA78291B56C}">
   <dimension ref="A1:E33"/>
   <sheetViews>
@@ -3413,7 +4086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9583AA52-5F44-4083-8962-4161C00EA6CA}">
   <dimension ref="A1:E33"/>
   <sheetViews>
@@ -3838,7 +4511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F1528E-0B9C-4CD2-89EB-8FFD151EF771}">
   <dimension ref="A1:E24"/>
   <sheetViews>
@@ -6103,11 +6776,562 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2703B7C7-6FE4-489B-A4A6-86279E170CB0}">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="4" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>596</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f t="shared" ref="A3:A34" si="0">ROW()-1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>598</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>598</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>598</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2966FB6C-C3F7-40CD-A351-BF1800F7F8C4}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6578,12 +7802,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0740C1D-B203-4921-BA8D-9A25B3E64DAD}">
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6974,7 +8198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDD6866-97AD-42DA-9774-4678D1F72157}">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -7307,7 +8531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B821F370-0792-4A0C-900F-286BE5257D66}">
   <dimension ref="A1:E63"/>
   <sheetViews>
@@ -8275,7 +9499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CCAB88-15F1-429D-84DF-E1E5D4D0A493}">
   <dimension ref="A1:E156"/>
   <sheetViews>
@@ -10177,672 +11401,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A7EB63-AF35-4A34-A800-1BC5F8A1BD55}">
-  <dimension ref="A1:J53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <f t="shared" ref="A2:A33" si="0">ROW()-1</f>
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>501</v>
-      </c>
-      <c r="E2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>502</v>
-      </c>
-      <c r="E3">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>503</v>
-      </c>
-      <c r="E4">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>504</v>
-      </c>
-      <c r="E5">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>505</v>
-      </c>
-      <c r="E6">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>506</v>
-      </c>
-      <c r="E7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>507</v>
-      </c>
-      <c r="E8">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>508</v>
-      </c>
-      <c r="E9">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>457</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>473</v>
-      </c>
-      <c r="E11">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>489</v>
-      </c>
-      <c r="E12">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>458</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>474</v>
-      </c>
-      <c r="E14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>490</v>
-      </c>
-      <c r="E15">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>459</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>475</v>
-      </c>
-      <c r="E17">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>491</v>
-      </c>
-      <c r="E18">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>460</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>476</v>
-      </c>
-      <c r="E20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>492</v>
-      </c>
-      <c r="E21">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>461</v>
-      </c>
-      <c r="E22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>477</v>
-      </c>
-      <c r="E23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>493</v>
-      </c>
-      <c r="E24">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>462</v>
-      </c>
-      <c r="E25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>478</v>
-      </c>
-      <c r="E26">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>494</v>
-      </c>
-      <c r="E27">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>463</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>479</v>
-      </c>
-      <c r="E29">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>495</v>
-      </c>
-      <c r="E30">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>464</v>
-      </c>
-      <c r="E31">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>480</v>
-      </c>
-      <c r="E32">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>496</v>
-      </c>
-      <c r="E33">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f t="shared" ref="A34:A53" si="1">ROW()-1</f>
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>465</v>
-      </c>
-      <c r="E34">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>481</v>
-      </c>
-      <c r="E35">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>466</v>
-      </c>
-      <c r="E36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>482</v>
-      </c>
-      <c r="E37">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>467</v>
-      </c>
-      <c r="E38">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>483</v>
-      </c>
-      <c r="E39">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>468</v>
-      </c>
-      <c r="E40">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>484</v>
-      </c>
-      <c r="E41">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>469</v>
-      </c>
-      <c r="E42">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>485</v>
-      </c>
-      <c r="E43">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>497</v>
-      </c>
-      <c r="E44">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>470</v>
-      </c>
-      <c r="E45">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>486</v>
-      </c>
-      <c r="E46">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>498</v>
-      </c>
-      <c r="E47">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>471</v>
-      </c>
-      <c r="E48">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>487</v>
-      </c>
-      <c r="E49">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>499</v>
-      </c>
-      <c r="E50">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>472</v>
-      </c>
-      <c r="E51">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>488</v>
-      </c>
-      <c r="E52">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>500</v>
-      </c>
-      <c r="E53">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:E53" xr:uid="{35A7EB63-AF35-4A34-A800-1BC5F8A1BD55}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E53">
-      <sortCondition ref="B1:B53"/>
-    </sortState>
-  </autoFilter>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>